<commit_message>
updated comment on effect
</commit_message>
<xml_diff>
--- a/debate/all_states_COVID_cases.xlsx
+++ b/debate/all_states_COVID_cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stk\Documents\GitHub\covid\debate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C87FC4A-F828-45B3-A49C-F7A3F154D6B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC6977F-B990-4BA0-AD12-6EB944570AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{E6A621CE-4E60-4BE2-8679-BF12EF115319}"/>
   </bookViews>
@@ -241,9 +241,6 @@
     <t>Slope being positive for both graphs menas the highly vaxed did worse</t>
   </si>
   <si>
-    <t>from the baseline which was highly negative.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> If the vaccines worked, the trend would have gotten MORE negative!</t>
   </si>
   <si>
@@ -350,6 +347,32 @@
   </si>
   <si>
     <t>From CDC vax</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">from the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pre-vaccine baseline which was highly negative</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -8771,8 +8794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4098E87C-088F-4243-BAF1-14D416AEB5B1}">
   <dimension ref="A1:AZ57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AJ52" sqref="AJ52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8788,22 +8811,22 @@
   <sheetData>
     <row r="1" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>56</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
@@ -8819,15 +8842,15 @@
       <c r="AJ1" s="1"/>
       <c r="AK1" s="1"/>
       <c r="AL1" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:52" x14ac:dyDescent="0.35">
       <c r="F2" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="W2" t="s">
         <v>60</v>
@@ -8847,7 +8870,7 @@
         <v>53</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
@@ -8857,7 +8880,7 @@
         <v>55</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L3" s="1">
         <v>2020</v>
@@ -9032,7 +9055,7 @@
         <v>12.895693084894885</v>
       </c>
       <c r="AE6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AF6" cm="1">
         <f t="array" ref="AF6:AG10">LINEST($I$4:$I$53, $F$4:$F$53, TRUE, TRUE)</f>
@@ -9042,10 +9065,10 @@
         <v>0.65662544377463494</v>
       </c>
       <c r="AH6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AR6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AS6" cm="1">
         <f t="array" ref="AS6:AT10">LINEST($R$4:$R$53, $F$4:$F$53, TRUE, TRUE)</f>
@@ -9055,7 +9078,7 @@
         <v>10.385338953950377</v>
       </c>
       <c r="AU6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:52" x14ac:dyDescent="0.35">
@@ -9108,7 +9131,7 @@
         <v>13.545581127940999</v>
       </c>
       <c r="AE7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AF7">
         <v>1.238979974026197E-3</v>
@@ -9117,7 +9140,7 @@
         <v>0.19022664414978174</v>
       </c>
       <c r="AR7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AS7">
         <v>1.4788628771790772E-2</v>
@@ -9176,7 +9199,7 @@
         <v>14.065369075399733</v>
       </c>
       <c r="AE8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AF8">
         <v>0.1534959276368793</v>
@@ -9185,7 +9208,7 @@
         <v>0.19931302596795067</v>
       </c>
       <c r="AR8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AS8">
         <v>1.8611858381314485E-2</v>
@@ -9418,14 +9441,14 @@
         <v>13.896558902430881</v>
       </c>
       <c r="AE12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AF12">
         <f>AF6-(1.96*AF7)</f>
         <v>1.2268637504347099E-3</v>
       </c>
       <c r="AR12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AS12">
         <f>AS6-(1.96*AS7)</f>
@@ -9482,14 +9505,14 @@
         <v>13.707656833232612</v>
       </c>
       <c r="AE13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AF13">
         <f>AF6+(1.96*AF7)</f>
         <v>6.0836652486174021E-3</v>
       </c>
       <c r="AR13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AS13">
         <f>AS6+(1.96*AS7)</f>
@@ -9896,7 +9919,7 @@
         <v>13.738123989568304</v>
       </c>
       <c r="AE21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AF21" cm="1">
         <f t="array" ref="AF21:AG25">LINEST($H$4:$H$53, $F$4:$F$53, TRUE, TRUE)</f>
@@ -9906,10 +9929,10 @@
         <v>-1.6795752894054017</v>
       </c>
       <c r="AH21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AR21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AS21" cm="1">
         <f t="array" ref="AS21:AT25">LINEST($Q$4:$Q$53, $F$4:$F$53, TRUE, TRUE)</f>
@@ -9919,7 +9942,7 @@
         <v>13.064905637071229</v>
       </c>
       <c r="AU21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -9972,7 +9995,7 @@
         <v>12.937114919075896</v>
       </c>
       <c r="AE22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AF22">
         <v>6.078351219375046E-3</v>
@@ -9982,7 +10005,7 @@
       </c>
       <c r="AH22"/>
       <c r="AR22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AS22">
         <v>1.0619289120457719E-2</v>
@@ -10042,7 +10065,7 @@
         <v>8.8318901610145577</v>
       </c>
       <c r="AE23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AF23">
         <v>0.24358816961527213</v>
@@ -10051,7 +10074,7 @@
         <v>0.97781610665807839</v>
       </c>
       <c r="AR23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AS23">
         <v>5.0238502119520703E-2</v>
@@ -10284,14 +10307,14 @@
         <v>6.7782278186785696</v>
       </c>
       <c r="AE27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AF27">
         <f>AF21-(1.96*AF22)</f>
         <v>1.1984090029077094E-2</v>
       </c>
       <c r="AR27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AS27">
         <f>AS21-(1.96*AS22)</f>
@@ -10348,14 +10371,14 @@
         <v>14.163024730472912</v>
       </c>
       <c r="AE28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AF28">
         <f>AF21+(1.96*AF22)</f>
         <v>3.5811226809027277E-2</v>
       </c>
       <c r="AR28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AS28">
         <f>AS21+(1.96*AS22)</f>
@@ -10812,7 +10835,7 @@
         <v>15.090853345588496</v>
       </c>
       <c r="AE37" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AF37" cm="1">
         <f t="array" ref="AF37:AG41">LINEST($J$4:$J$53, $F$4:$F$53, TRUE, TRUE)</f>
@@ -10822,10 +10845,10 @@
         <v>-2.5393905579987228</v>
       </c>
       <c r="AH37" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AR37" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AS37" cm="1">
         <f t="array" ref="AS37:AT41">LINEST($P$4:$P$53, $F$4:$F$53, TRUE, TRUE)</f>
@@ -10835,7 +10858,7 @@
         <v>13.833268555322178</v>
       </c>
       <c r="AU37" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:47" x14ac:dyDescent="0.35">
@@ -10888,7 +10911,7 @@
         <v>10.985595681817834</v>
       </c>
       <c r="AE38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AF38">
         <v>7.3187101926316146E-3</v>
@@ -10897,7 +10920,7 @@
         <v>1.1236773060382634</v>
       </c>
       <c r="AR38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AS38">
         <v>1.0978355385501411E-2</v>
@@ -10956,7 +10979,7 @@
         <v>13.559604955470423</v>
       </c>
       <c r="AE39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AF39">
         <v>0.27271131296919399</v>
@@ -10965,7 +10988,7 @@
         <v>1.1773509703596283</v>
       </c>
       <c r="AR39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AS39">
         <v>0.29680841565868893</v>
@@ -11198,7 +11221,7 @@
         <v>9.5847261044395662</v>
       </c>
       <c r="AE43" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AF43">
         <f>AF37-(1.96*AF38)</f>
@@ -11207,7 +11230,7 @@
       <c r="AG43"/>
       <c r="AH43"/>
       <c r="AR43" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AS43">
         <f>AS37-(1.96*AS38)</f>
@@ -11266,14 +11289,14 @@
         <v>10.287464749354426</v>
       </c>
       <c r="AE44" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AF44">
         <f>AF37+(1.96*AF38)</f>
         <v>4.5394080393687947E-2</v>
       </c>
       <c r="AR44" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AS44">
         <f>AS37+(1.96*AS38)</f>
@@ -11380,7 +11403,7 @@
         <v>11.377229195603697</v>
       </c>
       <c r="AE46" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="47" spans="1:47" x14ac:dyDescent="0.35">
@@ -11433,7 +11456,7 @@
         <v>12.954548009844411</v>
       </c>
       <c r="AE47" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:47" x14ac:dyDescent="0.35">
@@ -11586,7 +11609,7 @@
         <v>13.288330812072152</v>
       </c>
       <c r="V50" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="51" spans="1:36" x14ac:dyDescent="0.35">
@@ -11639,7 +11662,7 @@
         <v>14.258963750600548</v>
       </c>
       <c r="V51" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AJ51" s="1" t="s">
         <v>59</v>
@@ -11695,10 +11718,10 @@
         <v>16.706081043018191</v>
       </c>
       <c r="V52" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AJ52" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
     </row>
     <row r="53" spans="1:36" x14ac:dyDescent="0.35">
@@ -11751,7 +11774,7 @@
         <v>11.514480177370777</v>
       </c>
       <c r="AJ53" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -11769,28 +11792,28 @@
       </c>
       <c r="I54"/>
       <c r="V54" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:36" x14ac:dyDescent="0.35">
       <c r="V55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AJ55" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:36" x14ac:dyDescent="0.35">
       <c r="V56" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="57" spans="1:36" x14ac:dyDescent="0.35">
       <c r="V57" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ57" t="s">
         <v>85</v>
-      </c>
-      <c r="AJ57" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -11812,7 +11835,7 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.35">
@@ -11822,37 +11845,37 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added harvard line fit
</commit_message>
<xml_diff>
--- a/debate/all_states_COVID_cases.xlsx
+++ b/debate/all_states_COVID_cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stk\Documents\GitHub\covid\debate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC6977F-B990-4BA0-AD12-6EB944570AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80DBED2C-1020-4E37-9170-79720CB1294F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{E6A621CE-4E60-4BE2-8679-BF12EF115319}"/>
+    <workbookView xWindow="3240" yWindow="3660" windowWidth="30410" windowHeight="17220" xr2:uid="{E6A621CE-4E60-4BE2-8679-BF12EF115319}"/>
   </bookViews>
   <sheets>
     <sheet name="covid cases" sheetId="12" r:id="rId1"/>
@@ -8794,7 +8794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4098E87C-088F-4243-BAF1-14D416AEB5B1}">
   <dimension ref="A1:AZ57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AJ52" sqref="AJ52"/>
     </sheetView>
   </sheetViews>

</xml_diff>